<commit_message>
updated role location property name
</commit_message>
<xml_diff>
--- a/Data/testDataFactory.xlsx
+++ b/Data/testDataFactory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thuang4\Documents\GitHub\FAMO\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megankatsumi/FAMO/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83AB836-B44E-4D4D-B82C-A8E37E6C4E13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB35603-8845-1B4B-841B-7E103BAA6DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14120" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__readMe" sheetId="7" r:id="rId1"/>
@@ -665,7 +665,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -809,12 +809,6 @@
       <sz val="12"/>
       <color theme="1" tint="0.499984740745262"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1174,79 +1168,51 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1296,16 +1262,6 @@
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="52">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1511,6 +1467,16 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3358,15 +3324,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table5" displayName="Table5" ref="A1:I5" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table5" displayName="Table5" ref="A1:I5" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A1:I5" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="UID" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="UID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Activity Type"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Acting on" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Acting on" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Done by"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Date" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Time" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Date" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Time" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Interpretation Outcome"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Description Outcome"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Entity Number Outcome"/>
@@ -3376,11 +3342,11 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table81011" displayName="Table81011" ref="A1:B7" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table81011" displayName="Table81011" ref="A1:B7" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B7" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Entity Number" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Drawing Set Page Number" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Entity Number" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Drawing Set Page Number" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3434,12 +3400,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table810" displayName="Table810" ref="B2:D24" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table810" displayName="Table810" ref="B2:D24" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="B2:D24" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Drawing Tag UID" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Entity Number" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Drawing Set Page Number" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Drawing Tag UID" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Entity Number" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Drawing Set Page Number" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3457,19 +3423,19 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE8C41A2-7FCC-4A4D-84EF-128A5BC5A614}" name="Table6" displayName="Table6" ref="B2:D23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CE8C41A2-7FCC-4A4D-84EF-128A5BC5A614}" name="Table6" displayName="Table6" ref="B2:D23" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="B2:D23" xr:uid="{29421CFA-D5AA-4B07-9386-FF1EE054C66F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B08933A8-2602-476A-8C24-02C33ABC2493}" name="ETMS Role UID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{F5143272-340C-4F2B-B738-6850627429E7}" name="Entity Number" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{28FD2C0F-FD60-43A9-9C39-879B118D7AA6}" name="Description" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{B08933A8-2602-476A-8C24-02C33ABC2493}" name="ETMS Role UID" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{F5143272-340C-4F2B-B738-6850627429E7}" name="Entity Number" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{28FD2C0F-FD60-43A9-9C39-879B118D7AA6}" name="Description" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table7" displayName="Table7" ref="A1:D5" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table7" displayName="Table7" ref="A1:D5" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A1:D5" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="UID"/>
@@ -3482,16 +3448,16 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table4" displayName="Table4" ref="A1:I3" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table4" displayName="Table4" ref="A1:I3" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A1:I3" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="UID" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="UID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Activity Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Acting on Asset"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Acting on Role" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Acting on Role" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Done by"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Date" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Time" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Date" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Time" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="LCS Outcome"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Moved To"/>
   </tableColumns>
@@ -3776,24 +3742,24 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -3804,7 +3770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3815,7 +3781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3826,8 +3792,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3848,19 +3814,19 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.08984375" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" customWidth="1"/>
-    <col min="8" max="8" width="28.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -3876,103 +3842,103 @@
       <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="5">
         <v>44759</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>44760</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="6">
         <v>0.625</v>
       </c>
-      <c r="G3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="5">
         <v>44761</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>0.66666666666666696</v>
       </c>
       <c r="H4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>70</v>
       </c>
       <c r="D5" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="5">
         <v>44762</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="6">
         <v>0.70833333333333304</v>
       </c>
       <c r="I5" t="s">
@@ -3996,13 +3962,13 @@
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4010,7 +3976,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -4018,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4026,7 +3992,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4034,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4042,7 +4008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -4050,7 +4016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4075,47 +4041,47 @@
   <dimension ref="A2:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="35.6328125" customWidth="1"/>
-    <col min="4" max="4" width="81.36328125" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" customWidth="1"/>
-    <col min="7" max="7" width="99.7265625" customWidth="1"/>
-    <col min="8" max="8" width="11.08984375" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B2" s="28" t="b">
+      <c r="B2" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="C2" s="28" t="b">
+      <c r="C2" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="28" t="b">
+      <c r="D2" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="28" t="b">
+      <c r="E2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="28" t="b">
+      <c r="F2" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="28" t="b">
+      <c r="G2" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="28" t="b">
+      <c r="H2" s="18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4134,11 +4100,11 @@
       <c r="G3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>1181</v>
       </c>
@@ -4155,21 +4121,21 @@
       <c r="G4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>1182</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="10" t="s">
         <v>111</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="9">
         <v>1181</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -4178,21 +4144,21 @@
       <c r="G5" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>1183</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="11" t="s">
         <v>95</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="9">
         <v>1182</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -4201,21 +4167,21 @@
       <c r="G6" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>1184</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="11" t="s">
         <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="9">
         <v>1182</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -4224,21 +4190,21 @@
       <c r="G7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>1185</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="9">
         <v>1182</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -4247,159 +4213,159 @@
       <c r="G8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>1186</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>98</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="9">
         <v>1182</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>1187</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="9">
         <v>1182</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>1188</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E11" s="9">
         <v>1182</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>1189</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="9">
         <v>1182</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>1190</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="9">
         <v>1182</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>1191</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="9">
         <v>1182</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>1192</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="10" t="s">
         <v>113</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="9">
         <v>1181</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -4408,21 +4374,21 @@
       <c r="G15" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>1193</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="11" t="s">
         <v>114</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="9">
         <v>1192</v>
       </c>
       <c r="F16" s="2" t="s">
@@ -4431,21 +4397,21 @@
       <c r="G16" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>1194</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="11" t="s">
         <v>116</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="19">
+      <c r="E17" s="9">
         <v>1192</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -4454,21 +4420,21 @@
       <c r="G17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>1195</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="11" t="s">
         <v>118</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E18" s="19">
+      <c r="E18" s="9">
         <v>1192</v>
       </c>
       <c r="F18" s="2" t="s">
@@ -4477,145 +4443,145 @@
       <c r="G18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>1196</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="11" t="s">
         <v>120</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="9">
         <v>1192</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>1197</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="9">
         <v>1192</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>1198</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="9">
         <v>1192</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>1199</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="9">
         <v>1192</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H22" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>1200</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="9">
         <v>1192</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="14">
+      <c r="H23" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>1201</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="9">
         <v>1192</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H24" s="14">
+      <c r="H24" s="2">
         <v>3</v>
       </c>
     </row>
@@ -4642,18 +4608,18 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" customWidth="1"/>
-    <col min="5" max="5" width="34.6328125" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="16.453125" customWidth="1"/>
-    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -4679,7 +4645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -4702,7 +4668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>93620</v>
       </c>
@@ -4721,11 +4687,11 @@
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="9">
         <v>1182</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>93621</v>
       </c>
@@ -4741,14 +4707,14 @@
       <c r="F4" t="s">
         <v>196</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="9">
         <v>1183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>93622</v>
       </c>
@@ -4767,11 +4733,11 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="9">
         <v>1184</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>93623</v>
       </c>
@@ -4790,11 +4756,11 @@
       <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="9">
         <v>1185</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>93624</v>
       </c>
@@ -4813,11 +4779,11 @@
       <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="9">
         <v>1186</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>93625</v>
       </c>
@@ -4836,11 +4802,11 @@
       <c r="G8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="9">
         <v>1187</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>93626</v>
       </c>
@@ -4859,11 +4825,11 @@
       <c r="G9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="9">
         <v>1188</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>93627</v>
       </c>
@@ -4882,11 +4848,11 @@
       <c r="G10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="9">
         <v>1189</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>93628</v>
       </c>
@@ -4905,11 +4871,11 @@
       <c r="G11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="9">
         <v>1190</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>93629</v>
       </c>
@@ -4928,11 +4894,11 @@
       <c r="G12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="9">
         <v>1191</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>93630</v>
       </c>
@@ -4951,11 +4917,11 @@
       <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="9">
         <v>1192</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>93631</v>
       </c>
@@ -4974,11 +4940,11 @@
       <c r="G14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="9">
         <v>1193</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>93632</v>
       </c>
@@ -4997,11 +4963,11 @@
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="9">
         <v>1194</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>93633</v>
       </c>
@@ -5020,11 +4986,11 @@
       <c r="G16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="9">
         <v>1195</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>93634</v>
       </c>
@@ -5043,11 +5009,11 @@
       <c r="G17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="9">
         <v>1196</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>93635</v>
       </c>
@@ -5066,11 +5032,11 @@
       <c r="G18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="9">
         <v>1197</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>93636</v>
       </c>
@@ -5089,11 +5055,11 @@
       <c r="G19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="9">
         <v>1198</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>93637</v>
       </c>
@@ -5112,11 +5078,11 @@
       <c r="G20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="9">
         <v>1199</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>93638</v>
       </c>
@@ -5135,11 +5101,11 @@
       <c r="G21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="9">
         <v>1200</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>93639</v>
       </c>
@@ -5158,135 +5124,135 @@
       <c r="G22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H22" s="15">
+      <c r="H22" s="9">
         <v>1201</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="24">
+    <row r="23" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="15">
         <v>93640</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="15"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="24">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="15">
         <v>93641</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="15"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="24">
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B25" s="15">
         <v>93642</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="15"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="24">
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" s="15">
         <v>93643</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="15"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="24">
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="15">
         <v>93644</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G27" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H27" s="15"/>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="24">
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="15">
         <v>93645</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G28" s="27" t="s">
+      <c r="G28" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H28" s="15"/>
+      <c r="H28" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -5309,17 +5275,17 @@
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
-    <col min="3" max="3" width="20.453125" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.6328125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="7" max="7" width="50.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="50.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -5342,7 +5308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -5358,127 +5324,127 @@
       <c r="F2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="20">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="12">
         <v>968754</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="20">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="12">
         <v>968755</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="20">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="12">
         <v>968756</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="20">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="12">
         <v>968757</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="20">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="12">
         <v>968758</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="20">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="12">
         <v>968759</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5503,14 +5469,14 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -5524,8 +5490,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -5535,8 +5501,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="15">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="9">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5546,8 +5512,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="15">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5557,8 +5523,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="15">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5568,8 +5534,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="15">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5579,8 +5545,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="15">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5590,8 +5556,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="15">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5601,8 +5567,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="15">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5612,174 +5578,174 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="15">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="9">
         <v>8</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="9">
         <v>9</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="2" t="s">
         <v>101</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="15">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="9">
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="2" t="s">
         <v>102</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="15">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="9">
         <v>11</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="15">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="9">
         <v>12</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="15">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="9">
         <v>13</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="9">
         <v>14</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
+    <row r="17" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="9">
         <v>15</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="15">
+    <row r="18" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="9">
         <v>16</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="15">
+    <row r="19" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="9">
         <v>17</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="15">
+    <row r="20" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="9">
         <v>18</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="15">
+    <row r="21" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="9">
         <v>19</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="15">
+    <row r="22" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="9">
         <v>20</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="15">
+    <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="9">
         <v>21</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="15">
+    <row r="24" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B24" s="9">
         <v>22</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C24">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5801,13 +5767,13 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -5818,7 +5784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -5826,7 +5792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>19328</v>
       </c>
@@ -5834,7 +5800,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>373866</v>
       </c>
@@ -5842,7 +5808,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>442892</v>
       </c>
@@ -5850,7 +5816,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>845375</v>
       </c>
@@ -5858,7 +5824,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>348148</v>
       </c>
@@ -5866,7 +5832,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>881933</v>
       </c>
@@ -5874,7 +5840,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>227387</v>
       </c>
@@ -5882,7 +5848,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>301292</v>
       </c>
@@ -5890,7 +5856,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>532317</v>
       </c>
@@ -5898,7 +5864,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>356097</v>
       </c>
@@ -5906,7 +5872,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>803050</v>
       </c>
@@ -5914,7 +5880,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>100606</v>
       </c>
@@ -5922,7 +5888,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>958022</v>
       </c>
@@ -5930,7 +5896,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>922976</v>
       </c>
@@ -5938,7 +5904,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>480776</v>
       </c>
@@ -5946,7 +5912,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>297934</v>
       </c>
@@ -5954,7 +5920,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>761341</v>
       </c>
@@ -5962,7 +5928,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>2341</v>
       </c>
@@ -5970,7 +5936,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>360506</v>
       </c>
@@ -5978,7 +5944,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>880911</v>
       </c>
@@ -6005,14 +5971,14 @@
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="71.08984375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>198</v>
       </c>
@@ -6026,7 +5992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>92</v>
       </c>
@@ -6037,8 +6003,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="23">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B3" s="14">
         <v>23764</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -6048,8 +6014,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
         <v>23765</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -6059,8 +6025,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="14">
         <v>23766</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -6070,8 +6036,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="14">
         <v>23768</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6081,8 +6047,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="14">
         <v>23769</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6092,8 +6058,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="14">
         <v>23770</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6103,8 +6069,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="23">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="14">
         <v>23771</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6114,8 +6080,8 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="14">
         <v>23772</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6125,8 +6091,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="14">
         <v>23773</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6136,8 +6102,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="14">
         <v>23774</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6147,8 +6113,8 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="23">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="14">
         <v>23775</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6158,8 +6124,8 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="23">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="14">
         <v>23776</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6169,8 +6135,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="23">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B15" s="14">
         <v>23777</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6180,8 +6146,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="23">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
         <v>23778</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6191,8 +6157,8 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="23">
+    <row r="17" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="14">
         <v>23779</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6202,8 +6168,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="23">
+    <row r="18" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="14">
         <v>23780</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6213,8 +6179,8 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="23">
+    <row r="19" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="14">
         <v>23781</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -6224,8 +6190,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="23">
+    <row r="20" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B20" s="14">
         <v>23782</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -6235,8 +6201,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="23">
+    <row r="21" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B21" s="14">
         <v>23783</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -6246,8 +6212,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="23">
+    <row r="22" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B22" s="14">
         <v>23784</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -6257,8 +6223,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="23">
+    <row r="23" spans="2:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="B23" s="14">
         <v>23785</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -6268,140 +6234,140 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="12"/>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="12"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="12"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="12"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="12"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="12"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="12"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="12"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="12"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="12"/>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="12"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="12"/>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="12"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="12"/>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="12"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="12"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="12"/>
+      <c r="D50" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6420,29 +6386,29 @@
       <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" customWidth="1"/>
-    <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -6456,7 +6422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -6470,7 +6436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -6484,7 +6450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -6515,19 +6481,19 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="18.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="9.26953125" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" customWidth="1"/>
-    <col min="8" max="8" width="16.08984375" customWidth="1"/>
-    <col min="9" max="9" width="10.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -6546,18 +6512,18 @@
       <c r="F1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -6569,33 +6535,33 @@
       <c r="E2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="5">
         <v>44749</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="6">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="5">
         <v>44750</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>0.625</v>
       </c>
       <c r="H3" t="e">

</xml_diff>